<commit_message>
add match 31 and 41
</commit_message>
<xml_diff>
--- a/scoresheets/MATCH31.xlsx
+++ b/scoresheets/MATCH31.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t xml:space="preserve">Science Bros</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -852,7 +855,7 @@
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -1468,11 +1471,15 @@
       <c r="A3" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="46" t="n">
+        <v>13</v>
+      </c>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
       <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
+      <c r="F3" s="47" t="n">
+        <v>9</v>
+      </c>
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
@@ -1748,8 +1755,8 @@
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.80078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1811,7 +1818,9 @@
         <v>1</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="D3" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="13"/>
@@ -1834,7 +1843,9 @@
       <c r="B5" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="15" t="n">
+        <v>2</v>
+      </c>
       <c r="D5" s="16"/>
       <c r="E5" s="14"/>
       <c r="F5" s="15"/>
@@ -1847,7 +1858,9 @@
         <v>4</v>
       </c>
       <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="16" t="n">
+        <v>3</v>
+      </c>
       <c r="E6" s="14"/>
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
@@ -1858,21 +1871,25 @@
       <c r="B7" s="52" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="18" t="n">
+        <v>2</v>
+      </c>
       <c r="D7" s="19"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18"/>
       <c r="G7" s="19"/>
       <c r="H7" s="17"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="53" t="n">
         <v>10</v>
       </c>
       <c r="B8" s="54" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="22" t="n">
+        <v>2</v>
+      </c>
       <c r="D8" s="23"/>
       <c r="E8" s="21"/>
       <c r="F8" s="22"/>
@@ -1888,7 +1905,9 @@
       <c r="D9" s="26"/>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="H9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,13 +1916,15 @@
         <v>8</v>
       </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="E10" s="24"/>
       <c r="F10" s="25"/>
       <c r="G10" s="26"/>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="53"/>
       <c r="B11" s="55" t="n">
         <v>9</v>
@@ -1920,7 +1941,9 @@
       <c r="B12" s="56" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="28" t="n">
+        <v>2</v>
+      </c>
       <c r="D12" s="29"/>
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
@@ -1938,7 +1961,9 @@
       <c r="D13" s="13"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="13" t="n">
+        <v>2</v>
+      </c>
       <c r="H13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,7 +1972,9 @@
         <v>12</v>
       </c>
       <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="16" t="n">
+        <v>2</v>
+      </c>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
       <c r="G14" s="16"/>
@@ -1958,7 +1985,9 @@
       <c r="B15" s="51" t="n">
         <v>13</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="n">
+        <v>3</v>
+      </c>
       <c r="D15" s="16"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
@@ -1973,7 +2002,9 @@
       <c r="C16" s="15"/>
       <c r="D16" s="16"/>
       <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="15" t="n">
+        <v>2</v>
+      </c>
       <c r="G16" s="16"/>
       <c r="H16" s="14"/>
     </row>
@@ -1985,7 +2016,9 @@
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="18" t="s">
+        <v>23</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="17"/>
     </row>
@@ -1997,7 +2030,9 @@
         <v>16</v>
       </c>
       <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="E18" s="21"/>
       <c r="F18" s="22"/>
       <c r="G18" s="23"/>
@@ -2012,15 +2047,19 @@
       <c r="D19" s="26"/>
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="G19" s="26" t="n">
+        <v>2</v>
+      </c>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="53"/>
       <c r="B20" s="55" t="n">
         <v>18</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="25" t="n">
+        <v>3</v>
+      </c>
       <c r="D20" s="26"/>
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
@@ -2045,7 +2084,9 @@
         <v>20</v>
       </c>
       <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
+      <c r="D22" s="29" t="n">
+        <v>2</v>
+      </c>
       <c r="E22" s="27"/>
       <c r="F22" s="28"/>
       <c r="G22" s="29"/>
@@ -2085,7 +2126,9 @@
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="15" t="n">
+        <v>2</v>
+      </c>
       <c r="G25" s="16"/>
       <c r="H25" s="14"/>
     </row>
@@ -2098,7 +2141,9 @@
       <c r="D26" s="16"/>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="16" t="n">
+        <v>2</v>
+      </c>
       <c r="H26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2147,7 +2192,9 @@
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+      <c r="F30" s="25" t="n">
+        <v>2</v>
+      </c>
       <c r="G30" s="26"/>
       <c r="H30" s="24"/>
     </row>
@@ -2160,7 +2207,9 @@
       <c r="D31" s="26"/>
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="26" t="n">
+        <v>3</v>
+      </c>
       <c r="H31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2171,7 +2220,9 @@
       <c r="C32" s="28"/>
       <c r="D32" s="29"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="28" t="n">
+        <v>2</v>
+      </c>
       <c r="G32" s="29"/>
       <c r="H32" s="27"/>
     </row>
@@ -2182,27 +2233,27 @@
       <c r="B33" s="36"/>
       <c r="C33" s="37" t="n">
         <f aca="false">SUM(C3:C32)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D33" s="38" t="n">
         <f aca="false">SUM(D3:D32)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E33" s="40" t="n">
         <f aca="false">SUM(E3:E32)+C33+D33</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F33" s="37" t="n">
         <f aca="false">SUM(F3:F32)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G33" s="38" t="n">
         <f aca="false">SUM(G3:G32)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H33" s="59" t="n">
         <f aca="false">SUM(H3:H32)+F33+G33</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I33" s="48"/>
       <c r="J33" s="48"/>
@@ -2262,7 +2313,7 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2304,7 +2355,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="62"/>
       <c r="C3" s="63" t="n">
@@ -2340,12 +2391,12 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="64"/>
       <c r="C5" s="65" t="n">
         <f aca="false">Alphabet!B3</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
@@ -2353,7 +2404,7 @@
       <c r="G5" s="65"/>
       <c r="H5" s="65" t="n">
         <f aca="false">Alphabet!F3</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
@@ -2376,12 +2427,12 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="62" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="62"/>
       <c r="C7" s="63" t="n">
         <f aca="false">Lightning!E33</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="63"/>
@@ -2389,7 +2440,7 @@
       <c r="G7" s="63"/>
       <c r="H7" s="63" t="n">
         <f aca="false">Lightning!H33</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I7" s="63"/>
       <c r="J7" s="63"/>
@@ -2412,12 +2463,12 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="66" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="66"/>
       <c r="C9" s="43" t="n">
         <f aca="false">SUM(C3:G8)</f>
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -2425,7 +2476,7 @@
       <c r="G9" s="43"/>
       <c r="H9" s="44" t="n">
         <f aca="false">SUM(H3:L8)</f>
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2492,10 +2543,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="68" t="n">
         <v>3</v>
@@ -2511,15 +2562,15 @@
       </c>
       <c r="B2" s="71" t="n">
         <f aca="false">3*C2+2*D2</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C2" s="72" t="n">
         <f aca="false">COUNTIF(Category!C3:C32, "&gt;2")+COUNTIF(Lightning!C3:C32, "&gt;2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" s="73" t="n">
         <f aca="false">COUNTIFS(Category!C3:C32, "&gt;0",Category!C3:C32, "&lt;3" )+COUNTIFS(Lightning!C3:C32, "&gt;0",Lightning!C3:C32, "&lt;3" )</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2529,15 +2580,15 @@
       </c>
       <c r="B3" s="75" t="n">
         <f aca="false">3*C3+2*D3</f>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C3" s="76" t="n">
         <f aca="false">COUNTIF(Category!D3:D32, "&gt;2")+COUNTIF(Lightning!D3:D32, "&gt;2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="77" t="n">
         <f aca="false">COUNTIFS(Category!D3:D32, "&gt;0",Category!D3:D32, "&lt;3" )+COUNTIFS(Lightning!D3:D32, "&gt;0",Lightning!D3:D32, "&lt;3" )</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2547,7 +2598,7 @@
       </c>
       <c r="B4" s="75" t="n">
         <f aca="false">3*C4+2*D4</f>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" s="78" t="n">
         <f aca="false">COUNTIF(Category!F3:F32, "&gt;2")+COUNTIF(Lightning!F3:F32, "&gt;2")</f>
@@ -2555,7 +2606,7 @@
       </c>
       <c r="D4" s="77" t="n">
         <f aca="false">COUNTIFS(Category!F3:F32, "&gt;0",Category!F3:F32, "&lt;3" )+COUNTIFS(Lightning!F3:F32, "&gt;0",Lightning!F3:F32, "&lt;3" )</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2565,15 +2616,15 @@
       </c>
       <c r="B5" s="80" t="n">
         <f aca="false">3*C5+2*D5</f>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C5" s="81" t="n">
         <f aca="false">COUNTIF(Category!G3:G32,"&gt;2")+COUNTIF(Lightning!G3:G32,"&gt;2")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="82" t="n">
         <f aca="false">COUNTIFS(Category!G3:G32, "&gt;0",Category!G3:G32, "&lt;3" )+COUNTIFS(Lightning!G3:G32, "&gt;0",Lightning!G3:G32, "&lt;3" )</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2602,10 +2653,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="29.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" s="68" t="n">
         <v>3</v>

</xml_diff>